<commit_message>
começo do dia 19, ultima edição de xlsx e comeco de csv
Signed-off-by: fdeodato11 <fdeodato11@gmail.com>
</commit_message>
<xml_diff>
--- a/testes/Controlede_Contas_TI_mensal.xlsx
+++ b/testes/Controlede_Contas_TI_mensal.xlsx
@@ -1,32 +1,152 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CONTAS\contas\testes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="1215" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Hi Excel!</t>
-  </si>
-  <si>
-    <t>second row</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+  <si>
+    <t>Cód. Forn</t>
+  </si>
+  <si>
+    <t>Fornecedores</t>
+  </si>
+  <si>
+    <t>Vencimento</t>
+  </si>
+  <si>
+    <t>Valores Ref.</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>B00922</t>
+  </si>
+  <si>
+    <t>Vivo Assinatura Mensal</t>
+  </si>
+  <si>
+    <t>GBR036</t>
+  </si>
+  <si>
+    <t>Vivo 3G</t>
+  </si>
+  <si>
+    <t>B02456</t>
+  </si>
+  <si>
+    <t>Vivo IP Dedicado</t>
+  </si>
+  <si>
+    <t>Vivo Monitora</t>
+  </si>
+  <si>
+    <t>B01958</t>
+  </si>
+  <si>
+    <t>Claro 3G</t>
+  </si>
+  <si>
+    <t>B00324</t>
+  </si>
+  <si>
+    <t>Embratel Vipphone</t>
+  </si>
+  <si>
+    <t>Embratel Link Internet</t>
+  </si>
+  <si>
+    <t>Unify (Siemens)</t>
+  </si>
+  <si>
+    <t>GBR145</t>
+  </si>
+  <si>
+    <t>B00665</t>
+  </si>
+  <si>
+    <t>Nitromidia</t>
+  </si>
+  <si>
+    <t>GBR137</t>
+  </si>
+  <si>
+    <t>B00709</t>
+  </si>
+  <si>
+    <t>Planus Taxa Fixa</t>
+  </si>
+  <si>
+    <t>GBR139</t>
+  </si>
+  <si>
+    <t>B01520</t>
+  </si>
+  <si>
+    <t>Konics</t>
+  </si>
+  <si>
+    <t>B02183</t>
+  </si>
+  <si>
+    <t>Engineering  (ENGDB)</t>
+  </si>
+  <si>
+    <t>GBR090</t>
+  </si>
+  <si>
+    <t>B02229</t>
+  </si>
+  <si>
+    <t>DirectNet  (NeoVia)</t>
+  </si>
+  <si>
+    <t>B02502</t>
+  </si>
+  <si>
+    <t>Straight</t>
+  </si>
+  <si>
+    <t>Recebido</t>
+  </si>
+  <si>
+    <t>Requisição</t>
+  </si>
+  <si>
+    <t>Pago</t>
+  </si>
+  <si>
+    <t>Vivo Movel</t>
+  </si>
+  <si>
+    <t>Planus Taxa Variavel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +154,101 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -51,23 +256,376 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="60% - Ênfase2" xfId="2" builtinId="36"/>
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +667,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +699,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +751,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,24 +944,349 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="36">
+        <v>43009</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10">
+        <v>27</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="13">
+        <v>25</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="37"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="37"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="13">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="17">
+        <v>15</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="13">
+        <v>15</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13">
+        <v>24</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="24">
+        <v>25</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="17">
+        <v>25</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="13">
+        <v>15</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="13">
+        <v>14</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="13">
+        <v>14</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="29">
+        <v>7</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44">
+        <v>11359411</v>
+      </c>
+      <c r="H15" s="43"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="21">
+        <v>9</v>
+      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="13">
+        <v>11</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="13">
+        <v>15</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="45"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>